<commit_message>
Zoe provided an updated marker gene list
</commit_message>
<xml_diff>
--- a/data/marker_genes/Genes for violin plots Hbo1 retina ECs.xlsx
+++ b/data/marker_genes/Genes for violin plots Hbo1 retina ECs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grant.z/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/grant.z/Lab work/scRNA-seq/Further analysis for Pete/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7592AE5-F51F-1744-B8C8-60766F7B0BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229BA9A-FE72-BB4C-8455-B0A2FD675D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="900" windowWidth="25440" windowHeight="14560" xr2:uid="{013309CD-3BD7-3449-81EE-913BC31C6BF8}"/>
+    <workbookView xWindow="35380" yWindow="9500" windowWidth="25440" windowHeight="14520" xr2:uid="{013309CD-3BD7-3449-81EE-913BC31C6BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -39,18 +33,12 @@
     <t>Endothelial identity</t>
   </si>
   <si>
-    <t>Sox16</t>
-  </si>
-  <si>
     <t>Gja4</t>
   </si>
   <si>
     <t>Vegfc</t>
   </si>
   <si>
-    <t>Sma3g</t>
-  </si>
-  <si>
     <t>Cxcl12</t>
   </si>
   <si>
@@ -220,6 +208,12 @@
   </si>
   <si>
     <t>Ccnd3</t>
+  </si>
+  <si>
+    <t>Sox17</t>
+  </si>
+  <si>
+    <t>Sema3g</t>
   </si>
 </sst>
 </file>
@@ -288,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,6 +295,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +613,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -636,442 +631,442 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>